<commit_message>
Alguns DSS bem como pequenos erros
</commit_message>
<xml_diff>
--- a/Modelos UML/Descrição UseCases/ListadeCarrosComprados.xlsx
+++ b/Modelos UML/Descrição UseCases/ListadeCarrosComprados.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pmcca\Documents\3º Ano\DSS\Trabalho\DSS\DSS\UseCase\Descrição UseCases\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pmcca\Documents\3º Ano\DSS\Trabalho\DSS\DSS\Modelos UML\Descrição UseCases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A26CA738-148C-4868-A197-1153F845C7EC}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BF6A9B9-E4E8-4B33-97DD-72701C1A68AC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7485" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Actor input</t>
   </si>
@@ -58,22 +58,19 @@
     <t>Registado no Sistema</t>
   </si>
   <si>
-    <t>1.&lt;&lt;include&gt;&gt; Fazer Login</t>
-  </si>
-  <si>
-    <t>2. Mostra Menu de opções</t>
-  </si>
-  <si>
-    <t>3. Seleciona historico de compras</t>
-  </si>
-  <si>
-    <t>4. Obtém informação</t>
-  </si>
-  <si>
-    <t>5. Mostra lista de carros comprados</t>
-  </si>
-  <si>
     <t>Verificou lista de carros comprados</t>
+  </si>
+  <si>
+    <t>1. Mostra Menu de opções</t>
+  </si>
+  <si>
+    <t>2. Seleciona historico de compras</t>
+  </si>
+  <si>
+    <t>3. Obtém informação</t>
+  </si>
+  <si>
+    <t>4. Mostra lista de carros comprados</t>
   </si>
 </sst>
 </file>
@@ -589,10 +586,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:D11"/>
+  <dimension ref="B1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -636,7 +633,7 @@
         <v>6</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D5" s="11"/>
     </row>
@@ -653,36 +650,29 @@
     </row>
     <row r="7" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="13"/>
-      <c r="C7" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="1"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="8" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="13"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="1" t="s">
-        <v>11</v>
-      </c>
+      <c r="C8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" s="13"/>
-      <c r="C9" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" s="1"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="10" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" s="13"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="13"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="2" t="s">
+      <c r="C10" s="4"/>
+      <c r="D10" s="2" t="s">
         <v>14</v>
       </c>
     </row>
@@ -692,7 +682,7 @@
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="C5:D5"/>
-    <mergeCell ref="B6:B11"/>
+    <mergeCell ref="B6:B10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>